<commit_message>
imported Norwegian and Danish data with temporary dummy column mappings
</commit_message>
<xml_diff>
--- a/raw_data/English_WS/EnglishWS_Byers.xlsx
+++ b/raw_data/English_WS/EnglishWS_Byers.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14686" uniqueCount="1212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14674" uniqueCount="1213">
   <si>
     <t>Kitty sleep</t>
   </si>
@@ -3790,6 +3790,9 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>word_ending</t>
   </si>
 </sst>
 </file>
@@ -3884,8 +3887,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3995,7 +4004,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4021,6 +4030,9 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4046,6 +4058,9 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -39366,8 +39381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E806"/>
   <sheetViews>
-    <sheetView topLeftCell="A679" workbookViewId="0">
-      <selection activeCell="D695" sqref="D695"/>
+    <sheetView topLeftCell="A753" workbookViewId="0">
+      <selection activeCell="D769" sqref="D769"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -50526,10 +50541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -50615,19 +50630,24 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="8" t="s">
-        <v>971</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>973</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>974</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>974</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="8" t="s">
         <v>973</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -50635,151 +50655,103 @@
         <v>973</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="8" t="s">
-        <v>973</v>
+        <v>1107</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
-        <v>973</v>
+        <v>1107</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="8" t="s">
-        <v>973</v>
+        <v>1107</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="8" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>976</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>976</v>
-      </c>
+        <v>972</v>
+      </c>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
-        <v>1107</v>
+        <v>1212</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>974</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>974</v>
-      </c>
+        <v>972</v>
+      </c>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>1107</v>
+        <v>978</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>975</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>975</v>
-      </c>
+        <v>974</v>
+      </c>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="8" t="s">
-        <v>1107</v>
+        <v>978</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>976</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>976</v>
-      </c>
+        <v>975</v>
+      </c>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
-        <v>977</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+        <v>979</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="8" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>974</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="8" t="s">
-        <v>978</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>975</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="8" t="s">
-        <v>978</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>976</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="8" t="s">
-        <v>979</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="8" t="s">
-        <v>979</v>
-      </c>
-      <c r="B26" s="8" t="s">
         <v>981</v>
       </c>
     </row>

</xml_diff>

<commit_message>
imported Thal datasets and fixed English WS mapping discrepancy
</commit_message>
<xml_diff>
--- a/raw_data/English_WS/EnglishWS_Byers.xlsx
+++ b/raw_data/English_WS/EnglishWS_Byers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39381,8 +39381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E806"/>
   <sheetViews>
-    <sheetView topLeftCell="A753" workbookViewId="0">
-      <selection activeCell="D769" sqref="D769"/>
+    <sheetView tabSelected="1" topLeftCell="A748" workbookViewId="0">
+      <selection activeCell="D767" sqref="D767"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -49478,7 +49478,7 @@
         <v>992</v>
       </c>
       <c r="D724" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="725" spans="1:4">
@@ -49490,7 +49490,7 @@
         <v>992</v>
       </c>
       <c r="D725" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="726" spans="1:4">
@@ -49502,7 +49502,7 @@
         <v>992</v>
       </c>
       <c r="D726" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="727" spans="1:4">
@@ -49514,7 +49514,7 @@
         <v>992</v>
       </c>
       <c r="D727" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="728" spans="1:4">
@@ -49526,7 +49526,7 @@
         <v>992</v>
       </c>
       <c r="D728" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="729" spans="1:4">
@@ -49538,7 +49538,7 @@
         <v>992</v>
       </c>
       <c r="D729" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="730" spans="1:4">
@@ -49550,7 +49550,7 @@
         <v>992</v>
       </c>
       <c r="D730" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="731" spans="1:4">
@@ -49562,7 +49562,7 @@
         <v>992</v>
       </c>
       <c r="D731" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="732" spans="1:4">
@@ -49574,7 +49574,7 @@
         <v>992</v>
       </c>
       <c r="D732" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="733" spans="1:4">
@@ -49586,7 +49586,7 @@
         <v>992</v>
       </c>
       <c r="D733" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="734" spans="1:4">
@@ -49598,7 +49598,7 @@
         <v>992</v>
       </c>
       <c r="D734" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="735" spans="1:4">
@@ -49610,7 +49610,7 @@
         <v>992</v>
       </c>
       <c r="D735" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="736" spans="1:4">
@@ -49622,7 +49622,7 @@
         <v>992</v>
       </c>
       <c r="D736" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="737" spans="1:5">
@@ -49634,7 +49634,7 @@
         <v>992</v>
       </c>
       <c r="D737" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="738" spans="1:5">
@@ -49646,7 +49646,7 @@
         <v>992</v>
       </c>
       <c r="D738" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="739" spans="1:5">
@@ -49658,7 +49658,7 @@
         <v>992</v>
       </c>
       <c r="D739" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="740" spans="1:5">
@@ -49670,7 +49670,7 @@
         <v>992</v>
       </c>
       <c r="D740" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="741" spans="1:5">
@@ -49682,7 +49682,7 @@
         <v>992</v>
       </c>
       <c r="D741" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="742" spans="1:5">
@@ -49694,7 +49694,7 @@
         <v>992</v>
       </c>
       <c r="D742" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="743" spans="1:5">
@@ -49706,7 +49706,7 @@
         <v>992</v>
       </c>
       <c r="D743" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="744" spans="1:5">
@@ -49718,7 +49718,7 @@
         <v>992</v>
       </c>
       <c r="D744" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E744" s="18"/>
     </row>
@@ -49731,7 +49731,7 @@
         <v>992</v>
       </c>
       <c r="D745" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E745" s="18"/>
     </row>
@@ -49744,7 +49744,7 @@
         <v>992</v>
       </c>
       <c r="D746" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E746" s="18"/>
     </row>
@@ -49757,7 +49757,7 @@
         <v>992</v>
       </c>
       <c r="D747" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E747" s="18"/>
     </row>
@@ -49770,7 +49770,7 @@
         <v>992</v>
       </c>
       <c r="D748" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E748" s="18"/>
     </row>
@@ -49783,7 +49783,7 @@
         <v>992</v>
       </c>
       <c r="D749" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E749" s="18"/>
     </row>
@@ -49796,7 +49796,7 @@
         <v>992</v>
       </c>
       <c r="D750" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E750" s="18"/>
     </row>
@@ -49809,7 +49809,7 @@
         <v>992</v>
       </c>
       <c r="D751" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E751" s="18"/>
     </row>
@@ -49822,7 +49822,7 @@
         <v>992</v>
       </c>
       <c r="D752" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E752" s="18"/>
     </row>
@@ -49835,7 +49835,7 @@
         <v>992</v>
       </c>
       <c r="D753" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E753" s="18"/>
     </row>
@@ -49848,7 +49848,7 @@
         <v>992</v>
       </c>
       <c r="D754" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E754" s="18"/>
     </row>
@@ -49861,7 +49861,7 @@
         <v>992</v>
       </c>
       <c r="D755" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E755" s="18"/>
     </row>
@@ -49874,7 +49874,7 @@
         <v>992</v>
       </c>
       <c r="D756" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E756" s="18"/>
     </row>
@@ -49887,7 +49887,7 @@
         <v>992</v>
       </c>
       <c r="D757" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E757" s="18"/>
     </row>
@@ -49900,7 +49900,7 @@
         <v>992</v>
       </c>
       <c r="D758" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E758" s="18"/>
     </row>
@@ -49913,7 +49913,7 @@
         <v>992</v>
       </c>
       <c r="D759" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E759" s="18"/>
     </row>
@@ -49926,7 +49926,7 @@
         <v>992</v>
       </c>
       <c r="D760" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E760" s="18"/>
     </row>
@@ -49939,7 +49939,7 @@
         <v>992</v>
       </c>
       <c r="D761" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E761" s="18"/>
     </row>
@@ -49952,7 +49952,7 @@
         <v>992</v>
       </c>
       <c r="D762" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E762" s="18"/>
     </row>
@@ -49965,7 +49965,7 @@
         <v>992</v>
       </c>
       <c r="D763" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E763" s="18"/>
     </row>
@@ -49978,7 +49978,7 @@
         <v>992</v>
       </c>
       <c r="D764" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E764" s="18"/>
     </row>
@@ -49991,7 +49991,7 @@
         <v>992</v>
       </c>
       <c r="D765" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E765" s="18"/>
     </row>
@@ -50004,7 +50004,7 @@
         <v>992</v>
       </c>
       <c r="D766" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E766" s="18"/>
     </row>
@@ -50017,7 +50017,7 @@
         <v>992</v>
       </c>
       <c r="D767" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E767" s="18"/>
     </row>
@@ -50030,7 +50030,7 @@
         <v>992</v>
       </c>
       <c r="D768" s="14" t="s">
-        <v>977</v>
+        <v>1212</v>
       </c>
       <c r="E768" s="18"/>
     </row>
@@ -50543,7 +50543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>